<commit_message>
spreadsheets: Update project spreadsheet
Remove grant tab https://github.com/INDIGO-Initiative/indigo-data-standard/issues/23
Fix ENUM https://github.com/INDIGO-Initiative/indigo-data-standard/issues/39

Update to latest schema
</commit_message>
<xml_diff>
--- a/indigo/spreadsheetform_guides/project_v012.xlsx
+++ b/indigo/spreadsheetform_guides/project_v012.xlsx
@@ -17,10 +17,10 @@
     <sheet name="Service Provisions" sheetId="7" state="visible" r:id="rId8"/>
     <sheet name="Outcome Payment Commitments" sheetId="8" state="visible" r:id="rId9"/>
     <sheet name="Investments" sheetId="9" state="visible" r:id="rId10"/>
-    <sheet name="Intermediary services" sheetId="10" state="visible" r:id="rId11"/>
-    <sheet name="Outcome Metrics" sheetId="11" state="visible" r:id="rId12"/>
-    <sheet name="Outcome Pricing" sheetId="12" state="visible" r:id="rId13"/>
-    <sheet name="Grants" sheetId="13" state="visible" r:id="rId14"/>
+    <sheet name="InvestmentsOrgRoleOptions" sheetId="10" state="hidden" r:id="rId11"/>
+    <sheet name="Intermediary services" sheetId="11" state="visible" r:id="rId12"/>
+    <sheet name="Outcome Metrics" sheetId="12" state="visible" r:id="rId13"/>
+    <sheet name="Outcome Pricing" sheetId="13" state="visible" r:id="rId14"/>
     <sheet name="Transactions" sheetId="14" state="visible" r:id="rId15"/>
     <sheet name="Technical Assistance" sheetId="15" state="visible" r:id="rId16"/>
     <sheet name="Technical Assistance Details" sheetId="16" state="visible" r:id="rId17"/>
@@ -42,7 +42,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1012" uniqueCount="833">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="978" uniqueCount="816">
   <si>
     <t xml:space="preserve">INDIGO Project ID</t>
   </si>
@@ -1071,6 +1071,33 @@
   </si>
   <si>
     <t xml:space="preserve">SPREADSHEETFORM:DOWN:investments:status</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Nonprofit/NGO</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Foundation/Philanthropist</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Government/Public Sector/Public Bank</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Multilateral/Bilateral/Intergovernmental Financial Institution</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Corporate Giving</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Investment Fund</t>
+  </si>
+  <si>
+    <t xml:space="preserve">High Net Worth Individual/Family Office/Private Bank</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Impact Investor</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Commercial</t>
   </si>
   <si>
     <t xml:space="preserve">Other Role 
@@ -1255,121 +1282,35 @@
     <t xml:space="preserve">SPREADSHEETFORM:DOWN:outcome_pricings:status</t>
   </si>
   <si>
-    <t xml:space="preserve">Amount Applied For</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Amount Awarded</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Amount Disbursed</t>
-  </si>
-  <si>
-    <t xml:space="preserve">360 Giving Identifier</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Title</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Award Date</t>
+    <t xml:space="preserve">Investment ID</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Grant ID</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Date</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Sending
+Organisation</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Receiving 
+Organisation</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Transaction 
+Type</t>
+  </si>
+  <si>
+    <t xml:space="preserve">In
+Sandboxes?</t>
   </si>
   <si>
     <t xml:space="preserve">Amount 
 In USD</t>
   </si>
   <si>
-    <t xml:space="preserve">Recipient
-Organisation</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Funding 
-Organisation</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Purpose</t>
-  </si>
-  <si>
-    <t xml:space="preserve">YYYY-MM</t>
-  </si>
-  <si>
-    <t xml:space="preserve">SPREADSHEETFORM:DOWN:grants:id</t>
-  </si>
-  <si>
-    <t xml:space="preserve">SPREADSHEETFORM:DOWN:grants:360giving_id/value</t>
-  </si>
-  <si>
-    <t xml:space="preserve">SPREADSHEETFORM:DOWN:grants:title/value</t>
-  </si>
-  <si>
-    <t xml:space="preserve">SPREADSHEETFORM:DOWN:grants:award_date/value</t>
-  </si>
-  <si>
-    <t xml:space="preserve">SPREADSHEETFORM:DOWN:grants:currency/value</t>
-  </si>
-  <si>
-    <t xml:space="preserve">SPREADSHEETFORM:DOWN:grants:amount_applied_for/amount/value</t>
-  </si>
-  <si>
-    <t xml:space="preserve">SPREADSHEETFORM:DOWN:grants:amount_applied_for/amount_usd/value</t>
-  </si>
-  <si>
-    <t xml:space="preserve">SPREADSHEETFORM:DOWN:grants:amount_awarded/amount/value</t>
-  </si>
-  <si>
-    <t xml:space="preserve">SPREADSHEETFORM:DOWN:grants:amount_awarded/amount_usd/value</t>
-  </si>
-  <si>
-    <t xml:space="preserve">SPREADSHEETFORM:DOWN:grants:amount_disbursed/amount/value</t>
-  </si>
-  <si>
-    <t xml:space="preserve">SPREADSHEETFORM:DOWN:grants:amount_disbursed/amount_usd/value</t>
-  </si>
-  <si>
-    <t xml:space="preserve">SPREADSHEETFORM:DOWN:grants:recipient_organisation_id/value</t>
-  </si>
-  <si>
-    <t xml:space="preserve">SPREADSHEETFORM:DOWN:grants:funding_organisation_id/value</t>
-  </si>
-  <si>
-    <t xml:space="preserve">SPREADSHEETFORM:DOWN:grants:description/value</t>
-  </si>
-  <si>
-    <t xml:space="preserve">SPREADSHEETFORM:DOWN:grants:purpose/value</t>
-  </si>
-  <si>
-    <t xml:space="preserve">SPREADSHEETFORM:DOWN:grants:source_ids</t>
-  </si>
-  <si>
-    <t xml:space="preserve">SPREADSHEETFORM:DOWN:grants:notes</t>
-  </si>
-  <si>
-    <t xml:space="preserve">SPREADSHEETFORM:DOWN:grants:status</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Investment ID</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Grant ID</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Date</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Sending
-Organisation</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Receiving 
-Organisation</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Transaction 
-Type</t>
-  </si>
-  <si>
-    <t xml:space="preserve">In
-Sandboxes?</t>
-  </si>
-  <si>
     <t xml:space="preserve">SPREADSHEETFORM:DOWN:transactions:investment_id/value</t>
   </si>
   <si>
@@ -1410,6 +1351,9 @@
   </si>
   <si>
     <t xml:space="preserve">SPREADSHEETFORM:DOWN:transactions:sandboxes</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Title</t>
   </si>
   <si>
     <t xml:space="preserve">Period Start</t>
@@ -1426,6 +1370,9 @@
     <t xml:space="preserve">Recipient 
 Organisation 
 Id</t>
+  </si>
+  <si>
+    <t xml:space="preserve">YYYY-MM</t>
   </si>
   <si>
     <t xml:space="preserve">SPREADSHEETFORM:DOWN:technical_assistances:id</t>
@@ -2952,6 +2899,79 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
+  <dimension ref="A1:A9"/>
+  <sheetViews>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <cols>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="50.15"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1025" min="2" style="0" width="11.52"/>
+  </cols>
+  <sheetData>
+    <row r="1" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="8" t="s">
+        <v>340</v>
+      </c>
+    </row>
+    <row r="2" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="8" t="s">
+        <v>341</v>
+      </c>
+    </row>
+    <row r="3" customFormat="false" ht="46.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="8" t="s">
+        <v>342</v>
+      </c>
+    </row>
+    <row r="4" customFormat="false" ht="68.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="8" t="s">
+        <v>343</v>
+      </c>
+    </row>
+    <row r="5" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="8" t="s">
+        <v>344</v>
+      </c>
+    </row>
+    <row r="6" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A6" s="8" t="s">
+        <v>345</v>
+      </c>
+    </row>
+    <row r="7" customFormat="false" ht="68.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A7" s="8" t="s">
+        <v>346</v>
+      </c>
+    </row>
+    <row r="8" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A8" s="8" t="s">
+        <v>347</v>
+      </c>
+    </row>
+    <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A9" s="8" t="s">
+        <v>348</v>
+      </c>
+    </row>
+  </sheetData>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
+  </headerFooter>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
   <dimension ref="A1:F32"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
@@ -2990,7 +3010,7 @@
         <v>265</v>
       </c>
       <c r="C3" s="10" t="s">
-        <v>340</v>
+        <v>349</v>
       </c>
       <c r="D3" s="11" t="s">
         <v>189</v>
@@ -3004,22 +3024,22 @@
     </row>
     <row r="4" customFormat="false" ht="87" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="12" t="s">
-        <v>341</v>
+        <v>350</v>
       </c>
       <c r="B4" s="7" t="s">
-        <v>342</v>
+        <v>351</v>
       </c>
       <c r="C4" s="7" t="s">
-        <v>343</v>
+        <v>352</v>
       </c>
       <c r="D4" s="12" t="s">
-        <v>344</v>
+        <v>353</v>
       </c>
       <c r="E4" s="7" t="s">
-        <v>345</v>
+        <v>354</v>
       </c>
       <c r="F4" s="7" t="s">
-        <v>346</v>
+        <v>355</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3270,7 +3290,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
@@ -3337,46 +3357,46 @@
         <v>263</v>
       </c>
       <c r="B3" s="10" t="s">
-        <v>347</v>
+        <v>356</v>
       </c>
       <c r="C3" s="10" t="s">
-        <v>348</v>
+        <v>357</v>
       </c>
       <c r="D3" s="10" t="s">
-        <v>349</v>
+        <v>358</v>
       </c>
       <c r="E3" s="10" t="s">
-        <v>350</v>
+        <v>359</v>
       </c>
       <c r="F3" s="10" t="s">
-        <v>351</v>
+        <v>360</v>
       </c>
       <c r="G3" s="4" t="s">
-        <v>352</v>
+        <v>361</v>
       </c>
       <c r="H3" s="10" t="s">
-        <v>353</v>
+        <v>362</v>
       </c>
       <c r="I3" s="10" t="s">
-        <v>354</v>
+        <v>363</v>
       </c>
       <c r="J3" s="10" t="s">
-        <v>355</v>
+        <v>364</v>
       </c>
       <c r="K3" s="10" t="s">
-        <v>356</v>
+        <v>365</v>
       </c>
       <c r="L3" s="10" t="s">
-        <v>357</v>
+        <v>366</v>
       </c>
       <c r="M3" s="10" t="s">
-        <v>358</v>
+        <v>367</v>
       </c>
       <c r="N3" s="10" t="s">
-        <v>359</v>
+        <v>368</v>
       </c>
       <c r="O3" s="10" t="s">
-        <v>360</v>
+        <v>369</v>
       </c>
       <c r="P3" s="11" t="s">
         <v>189</v>
@@ -3390,58 +3410,58 @@
     </row>
     <row r="4" customFormat="false" ht="115.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="16" t="s">
-        <v>361</v>
+        <v>370</v>
       </c>
       <c r="B4" s="7" t="s">
-        <v>362</v>
+        <v>371</v>
       </c>
       <c r="C4" s="7" t="s">
-        <v>363</v>
+        <v>372</v>
       </c>
       <c r="D4" s="7" t="s">
-        <v>364</v>
+        <v>373</v>
       </c>
       <c r="E4" s="7" t="s">
-        <v>365</v>
+        <v>374</v>
       </c>
       <c r="F4" s="7" t="s">
-        <v>366</v>
+        <v>375</v>
       </c>
       <c r="G4" s="7" t="s">
-        <v>367</v>
+        <v>376</v>
       </c>
       <c r="H4" s="7" t="s">
-        <v>368</v>
+        <v>377</v>
       </c>
       <c r="I4" s="7" t="s">
-        <v>369</v>
+        <v>378</v>
       </c>
       <c r="J4" s="7" t="s">
-        <v>370</v>
+        <v>379</v>
       </c>
       <c r="K4" s="7" t="s">
-        <v>371</v>
+        <v>380</v>
       </c>
       <c r="L4" s="7" t="s">
-        <v>372</v>
+        <v>381</v>
       </c>
       <c r="M4" s="7" t="s">
-        <v>373</v>
+        <v>382</v>
       </c>
       <c r="N4" s="7" t="s">
-        <v>374</v>
+        <v>383</v>
       </c>
       <c r="O4" s="7" t="s">
-        <v>375</v>
+        <v>384</v>
       </c>
       <c r="P4" s="12" t="s">
-        <v>376</v>
+        <v>385</v>
       </c>
       <c r="Q4" s="7" t="s">
-        <v>377</v>
+        <v>386</v>
       </c>
       <c r="R4" s="7" t="s">
-        <v>378</v>
+        <v>387</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4044,7 +4064,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
@@ -4052,7 +4072,7 @@
   <dimension ref="A1:J33"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+      <selection pane="topLeft" activeCell="G3" activeCellId="0" sqref="G3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -4074,11 +4094,11 @@
       <c r="A2" s="11"/>
       <c r="B2" s="4"/>
       <c r="C2" s="4" t="s">
-        <v>379</v>
+        <v>388</v>
       </c>
       <c r="D2" s="4"/>
       <c r="E2" s="10" t="s">
-        <v>380</v>
+        <v>389</v>
       </c>
       <c r="F2" s="4"/>
       <c r="G2" s="4"/>
@@ -4090,7 +4110,7 @@
     </row>
     <row r="3" customFormat="false" ht="44" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="17" t="s">
-        <v>381</v>
+        <v>390</v>
       </c>
       <c r="B3" s="4" t="s">
         <v>285</v>
@@ -4105,10 +4125,10 @@
         <v>286</v>
       </c>
       <c r="F3" s="10" t="s">
-        <v>382</v>
+        <v>391</v>
       </c>
       <c r="G3" s="4" t="s">
-        <v>383</v>
+        <v>392</v>
       </c>
       <c r="H3" s="11" t="s">
         <v>189</v>
@@ -4134,34 +4154,34 @@
     </row>
     <row r="5" customFormat="false" ht="114.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="12" t="s">
-        <v>384</v>
+        <v>393</v>
       </c>
       <c r="B5" s="7" t="s">
-        <v>385</v>
+        <v>394</v>
       </c>
       <c r="C5" s="7" t="s">
-        <v>386</v>
+        <v>395</v>
       </c>
       <c r="D5" s="7" t="s">
-        <v>387</v>
+        <v>396</v>
       </c>
       <c r="E5" s="7" t="s">
-        <v>388</v>
+        <v>397</v>
       </c>
       <c r="F5" s="7" t="s">
-        <v>389</v>
+        <v>398</v>
       </c>
       <c r="G5" s="7" t="s">
-        <v>390</v>
+        <v>399</v>
       </c>
       <c r="H5" s="12" t="s">
-        <v>391</v>
+        <v>400</v>
       </c>
       <c r="I5" s="7" t="s">
-        <v>392</v>
+        <v>401</v>
       </c>
       <c r="J5" s="7" t="s">
-        <v>393</v>
+        <v>402</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4516,793 +4536,6 @@
     </dataValidation>
     <dataValidation allowBlank="true" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="B5:G33" type="none">
       <formula1>0</formula1>
-      <formula2>0</formula2>
-    </dataValidation>
-  </dataValidations>
-  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
-  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
-  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
-  <headerFooter differentFirst="false" differentOddEven="false">
-    <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
-    <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
-  </headerFooter>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <sheetPr filterMode="false">
-    <pageSetUpPr fitToPage="false"/>
-  </sheetPr>
-  <dimension ref="A2:R33"/>
-  <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
-  <cols>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="11.52"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="14.43"/>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="5" min="3" style="0" width="11.52"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="14.03"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="13.19"/>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="8" min="8" style="0" width="11.52"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="0" width="13.89"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="0" width="12.78"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="0" width="13.75"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="13" min="12" style="0" width="15.14"/>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1025" min="14" style="0" width="11.52"/>
-  </cols>
-  <sheetData>
-    <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="14"/>
-      <c r="B2" s="4"/>
-      <c r="C2" s="4"/>
-      <c r="D2" s="4"/>
-      <c r="E2" s="4"/>
-      <c r="F2" s="4" t="s">
-        <v>394</v>
-      </c>
-      <c r="G2" s="4"/>
-      <c r="H2" s="4" t="s">
-        <v>395</v>
-      </c>
-      <c r="I2" s="4"/>
-      <c r="J2" s="4" t="s">
-        <v>396</v>
-      </c>
-      <c r="K2" s="4"/>
-      <c r="L2" s="4"/>
-      <c r="M2" s="4"/>
-      <c r="N2" s="4"/>
-      <c r="O2" s="4"/>
-      <c r="P2" s="4" t="s">
-        <v>182</v>
-      </c>
-      <c r="Q2" s="4"/>
-      <c r="R2" s="4"/>
-    </row>
-    <row r="3" customFormat="false" ht="29.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="14" t="s">
-        <v>263</v>
-      </c>
-      <c r="B3" s="10" t="s">
-        <v>397</v>
-      </c>
-      <c r="C3" s="10" t="s">
-        <v>398</v>
-      </c>
-      <c r="D3" s="10" t="s">
-        <v>399</v>
-      </c>
-      <c r="E3" s="10" t="s">
-        <v>285</v>
-      </c>
-      <c r="F3" s="4" t="s">
-        <v>286</v>
-      </c>
-      <c r="G3" s="10" t="s">
-        <v>400</v>
-      </c>
-      <c r="H3" s="4" t="s">
-        <v>286</v>
-      </c>
-      <c r="I3" s="10" t="s">
-        <v>400</v>
-      </c>
-      <c r="J3" s="4" t="s">
-        <v>286</v>
-      </c>
-      <c r="K3" s="10" t="s">
-        <v>400</v>
-      </c>
-      <c r="L3" s="10" t="s">
-        <v>401</v>
-      </c>
-      <c r="M3" s="10" t="s">
-        <v>402</v>
-      </c>
-      <c r="N3" s="10" t="s">
-        <v>268</v>
-      </c>
-      <c r="O3" s="10" t="s">
-        <v>403</v>
-      </c>
-      <c r="P3" s="11" t="s">
-        <v>189</v>
-      </c>
-      <c r="Q3" s="4" t="s">
-        <v>25</v>
-      </c>
-      <c r="R3" s="4" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="4" customFormat="false" ht="15.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="14"/>
-      <c r="B4" s="10"/>
-      <c r="C4" s="10"/>
-      <c r="D4" s="10" t="s">
-        <v>404</v>
-      </c>
-      <c r="E4" s="10"/>
-      <c r="F4" s="10"/>
-      <c r="G4" s="10"/>
-      <c r="H4" s="10"/>
-      <c r="I4" s="10"/>
-      <c r="J4" s="10"/>
-      <c r="K4" s="10"/>
-      <c r="L4" s="4" t="s">
-        <v>263</v>
-      </c>
-      <c r="M4" s="4" t="s">
-        <v>263</v>
-      </c>
-      <c r="N4" s="10"/>
-      <c r="O4" s="10"/>
-      <c r="P4" s="11"/>
-      <c r="Q4" s="4"/>
-      <c r="R4" s="4"/>
-    </row>
-    <row r="5" customFormat="false" ht="115.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="16" t="s">
-        <v>405</v>
-      </c>
-      <c r="B5" s="7" t="s">
-        <v>406</v>
-      </c>
-      <c r="C5" s="7" t="s">
-        <v>407</v>
-      </c>
-      <c r="D5" s="7" t="s">
-        <v>408</v>
-      </c>
-      <c r="E5" s="7" t="s">
-        <v>409</v>
-      </c>
-      <c r="F5" s="7" t="s">
-        <v>410</v>
-      </c>
-      <c r="G5" s="7" t="s">
-        <v>411</v>
-      </c>
-      <c r="H5" s="7" t="s">
-        <v>412</v>
-      </c>
-      <c r="I5" s="7" t="s">
-        <v>413</v>
-      </c>
-      <c r="J5" s="7" t="s">
-        <v>414</v>
-      </c>
-      <c r="K5" s="7" t="s">
-        <v>415</v>
-      </c>
-      <c r="L5" s="7" t="s">
-        <v>416</v>
-      </c>
-      <c r="M5" s="7" t="s">
-        <v>417</v>
-      </c>
-      <c r="N5" s="7" t="s">
-        <v>418</v>
-      </c>
-      <c r="O5" s="7" t="s">
-        <v>419</v>
-      </c>
-      <c r="P5" s="12" t="s">
-        <v>420</v>
-      </c>
-      <c r="Q5" s="7" t="s">
-        <v>421</v>
-      </c>
-      <c r="R5" s="7" t="s">
-        <v>422</v>
-      </c>
-    </row>
-    <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="16"/>
-      <c r="B6" s="7"/>
-      <c r="C6" s="7"/>
-      <c r="D6" s="7"/>
-      <c r="E6" s="7"/>
-      <c r="F6" s="7"/>
-      <c r="G6" s="7"/>
-      <c r="H6" s="7"/>
-      <c r="I6" s="7"/>
-      <c r="J6" s="7"/>
-      <c r="K6" s="7"/>
-      <c r="L6" s="7"/>
-      <c r="M6" s="7"/>
-      <c r="N6" s="7"/>
-      <c r="O6" s="7"/>
-      <c r="P6" s="12"/>
-      <c r="Q6" s="7"/>
-      <c r="R6" s="7"/>
-    </row>
-    <row r="7" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="16"/>
-      <c r="B7" s="7"/>
-      <c r="C7" s="7"/>
-      <c r="D7" s="7"/>
-      <c r="E7" s="7"/>
-      <c r="F7" s="7"/>
-      <c r="G7" s="7"/>
-      <c r="H7" s="7"/>
-      <c r="I7" s="7"/>
-      <c r="J7" s="7"/>
-      <c r="K7" s="7"/>
-      <c r="L7" s="7"/>
-      <c r="M7" s="7"/>
-      <c r="N7" s="7"/>
-      <c r="O7" s="7"/>
-      <c r="P7" s="12"/>
-      <c r="Q7" s="7"/>
-      <c r="R7" s="7"/>
-    </row>
-    <row r="8" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="16"/>
-      <c r="B8" s="7"/>
-      <c r="C8" s="7"/>
-      <c r="D8" s="7"/>
-      <c r="E8" s="7"/>
-      <c r="F8" s="7"/>
-      <c r="G8" s="7"/>
-      <c r="H8" s="7"/>
-      <c r="I8" s="7"/>
-      <c r="J8" s="7"/>
-      <c r="K8" s="7"/>
-      <c r="L8" s="7"/>
-      <c r="M8" s="7"/>
-      <c r="N8" s="7"/>
-      <c r="O8" s="7"/>
-      <c r="P8" s="12"/>
-      <c r="Q8" s="7"/>
-      <c r="R8" s="7"/>
-    </row>
-    <row r="9" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="16"/>
-      <c r="B9" s="7"/>
-      <c r="C9" s="7"/>
-      <c r="D9" s="7"/>
-      <c r="E9" s="7"/>
-      <c r="F9" s="7"/>
-      <c r="G9" s="7"/>
-      <c r="H9" s="7"/>
-      <c r="I9" s="7"/>
-      <c r="J9" s="7"/>
-      <c r="K9" s="7"/>
-      <c r="L9" s="7"/>
-      <c r="M9" s="7"/>
-      <c r="N9" s="7"/>
-      <c r="O9" s="7"/>
-      <c r="P9" s="12"/>
-      <c r="Q9" s="7"/>
-      <c r="R9" s="7"/>
-    </row>
-    <row r="10" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A10" s="16"/>
-      <c r="B10" s="7"/>
-      <c r="C10" s="7"/>
-      <c r="D10" s="7"/>
-      <c r="E10" s="7"/>
-      <c r="F10" s="7"/>
-      <c r="G10" s="7"/>
-      <c r="H10" s="7"/>
-      <c r="I10" s="7"/>
-      <c r="J10" s="7"/>
-      <c r="K10" s="7"/>
-      <c r="L10" s="7"/>
-      <c r="M10" s="7"/>
-      <c r="N10" s="7"/>
-      <c r="O10" s="7"/>
-      <c r="P10" s="12"/>
-      <c r="Q10" s="7"/>
-      <c r="R10" s="7"/>
-    </row>
-    <row r="11" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A11" s="16"/>
-      <c r="B11" s="7"/>
-      <c r="C11" s="7"/>
-      <c r="D11" s="7"/>
-      <c r="E11" s="7"/>
-      <c r="F11" s="7"/>
-      <c r="G11" s="7"/>
-      <c r="H11" s="7"/>
-      <c r="I11" s="7"/>
-      <c r="J11" s="7"/>
-      <c r="K11" s="7"/>
-      <c r="L11" s="7"/>
-      <c r="M11" s="7"/>
-      <c r="N11" s="7"/>
-      <c r="O11" s="7"/>
-      <c r="P11" s="12"/>
-      <c r="Q11" s="7"/>
-      <c r="R11" s="7"/>
-    </row>
-    <row r="12" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A12" s="16"/>
-      <c r="B12" s="7"/>
-      <c r="C12" s="7"/>
-      <c r="D12" s="7"/>
-      <c r="E12" s="7"/>
-      <c r="F12" s="7"/>
-      <c r="G12" s="7"/>
-      <c r="H12" s="7"/>
-      <c r="I12" s="7"/>
-      <c r="J12" s="7"/>
-      <c r="K12" s="7"/>
-      <c r="L12" s="7"/>
-      <c r="M12" s="7"/>
-      <c r="N12" s="7"/>
-      <c r="O12" s="7"/>
-      <c r="P12" s="12"/>
-      <c r="Q12" s="7"/>
-      <c r="R12" s="7"/>
-    </row>
-    <row r="13" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A13" s="16"/>
-      <c r="B13" s="7"/>
-      <c r="C13" s="7"/>
-      <c r="D13" s="7"/>
-      <c r="E13" s="7"/>
-      <c r="F13" s="7"/>
-      <c r="G13" s="7"/>
-      <c r="H13" s="7"/>
-      <c r="I13" s="7"/>
-      <c r="J13" s="7"/>
-      <c r="K13" s="7"/>
-      <c r="L13" s="7"/>
-      <c r="M13" s="7"/>
-      <c r="N13" s="7"/>
-      <c r="O13" s="7"/>
-      <c r="P13" s="12"/>
-      <c r="Q13" s="7"/>
-      <c r="R13" s="7"/>
-    </row>
-    <row r="14" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A14" s="16"/>
-      <c r="B14" s="7"/>
-      <c r="C14" s="7"/>
-      <c r="D14" s="7"/>
-      <c r="E14" s="7"/>
-      <c r="F14" s="7"/>
-      <c r="G14" s="7"/>
-      <c r="H14" s="7"/>
-      <c r="I14" s="7"/>
-      <c r="J14" s="7"/>
-      <c r="K14" s="7"/>
-      <c r="L14" s="7"/>
-      <c r="M14" s="7"/>
-      <c r="N14" s="7"/>
-      <c r="O14" s="7"/>
-      <c r="P14" s="12"/>
-      <c r="Q14" s="7"/>
-      <c r="R14" s="7"/>
-    </row>
-    <row r="15" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A15" s="16"/>
-      <c r="B15" s="7"/>
-      <c r="C15" s="7"/>
-      <c r="D15" s="7"/>
-      <c r="E15" s="7"/>
-      <c r="F15" s="7"/>
-      <c r="G15" s="7"/>
-      <c r="H15" s="7"/>
-      <c r="I15" s="7"/>
-      <c r="J15" s="7"/>
-      <c r="K15" s="7"/>
-      <c r="L15" s="7"/>
-      <c r="M15" s="7"/>
-      <c r="N15" s="7"/>
-      <c r="O15" s="7"/>
-      <c r="P15" s="12"/>
-      <c r="Q15" s="7"/>
-      <c r="R15" s="7"/>
-    </row>
-    <row r="16" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A16" s="16"/>
-      <c r="B16" s="7"/>
-      <c r="C16" s="7"/>
-      <c r="D16" s="7"/>
-      <c r="E16" s="7"/>
-      <c r="F16" s="7"/>
-      <c r="G16" s="7"/>
-      <c r="H16" s="7"/>
-      <c r="I16" s="7"/>
-      <c r="J16" s="7"/>
-      <c r="K16" s="7"/>
-      <c r="L16" s="7"/>
-      <c r="M16" s="7"/>
-      <c r="N16" s="7"/>
-      <c r="O16" s="7"/>
-      <c r="P16" s="12"/>
-      <c r="Q16" s="7"/>
-      <c r="R16" s="7"/>
-    </row>
-    <row r="17" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A17" s="16"/>
-      <c r="B17" s="7"/>
-      <c r="C17" s="7"/>
-      <c r="D17" s="7"/>
-      <c r="E17" s="7"/>
-      <c r="F17" s="7"/>
-      <c r="G17" s="7"/>
-      <c r="H17" s="7"/>
-      <c r="I17" s="7"/>
-      <c r="J17" s="7"/>
-      <c r="K17" s="7"/>
-      <c r="L17" s="7"/>
-      <c r="M17" s="7"/>
-      <c r="N17" s="7"/>
-      <c r="O17" s="7"/>
-      <c r="P17" s="12"/>
-      <c r="Q17" s="7"/>
-      <c r="R17" s="7"/>
-    </row>
-    <row r="18" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A18" s="16"/>
-      <c r="B18" s="7"/>
-      <c r="C18" s="7"/>
-      <c r="D18" s="7"/>
-      <c r="E18" s="7"/>
-      <c r="F18" s="7"/>
-      <c r="G18" s="7"/>
-      <c r="H18" s="7"/>
-      <c r="I18" s="7"/>
-      <c r="J18" s="7"/>
-      <c r="K18" s="7"/>
-      <c r="L18" s="7"/>
-      <c r="M18" s="7"/>
-      <c r="N18" s="7"/>
-      <c r="O18" s="7"/>
-      <c r="P18" s="12"/>
-      <c r="Q18" s="7"/>
-      <c r="R18" s="7"/>
-    </row>
-    <row r="19" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A19" s="16"/>
-      <c r="B19" s="7"/>
-      <c r="C19" s="7"/>
-      <c r="D19" s="7"/>
-      <c r="E19" s="7"/>
-      <c r="F19" s="7"/>
-      <c r="G19" s="7"/>
-      <c r="H19" s="7"/>
-      <c r="I19" s="7"/>
-      <c r="J19" s="7"/>
-      <c r="K19" s="7"/>
-      <c r="L19" s="7"/>
-      <c r="M19" s="7"/>
-      <c r="N19" s="7"/>
-      <c r="O19" s="7"/>
-      <c r="P19" s="12"/>
-      <c r="Q19" s="7"/>
-      <c r="R19" s="7"/>
-    </row>
-    <row r="20" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A20" s="16"/>
-      <c r="B20" s="7"/>
-      <c r="C20" s="7"/>
-      <c r="D20" s="7"/>
-      <c r="E20" s="7"/>
-      <c r="F20" s="7"/>
-      <c r="G20" s="7"/>
-      <c r="H20" s="7"/>
-      <c r="I20" s="7"/>
-      <c r="J20" s="7"/>
-      <c r="K20" s="7"/>
-      <c r="L20" s="7"/>
-      <c r="M20" s="7"/>
-      <c r="N20" s="7"/>
-      <c r="O20" s="7"/>
-      <c r="P20" s="12"/>
-      <c r="Q20" s="7"/>
-      <c r="R20" s="7"/>
-    </row>
-    <row r="21" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A21" s="16"/>
-      <c r="B21" s="7"/>
-      <c r="C21" s="7"/>
-      <c r="D21" s="7"/>
-      <c r="E21" s="7"/>
-      <c r="F21" s="7"/>
-      <c r="G21" s="7"/>
-      <c r="H21" s="7"/>
-      <c r="I21" s="7"/>
-      <c r="J21" s="7"/>
-      <c r="K21" s="7"/>
-      <c r="L21" s="7"/>
-      <c r="M21" s="7"/>
-      <c r="N21" s="7"/>
-      <c r="O21" s="7"/>
-      <c r="P21" s="12"/>
-      <c r="Q21" s="7"/>
-      <c r="R21" s="7"/>
-    </row>
-    <row r="22" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A22" s="16"/>
-      <c r="B22" s="7"/>
-      <c r="C22" s="7"/>
-      <c r="D22" s="7"/>
-      <c r="E22" s="7"/>
-      <c r="F22" s="7"/>
-      <c r="G22" s="7"/>
-      <c r="H22" s="7"/>
-      <c r="I22" s="7"/>
-      <c r="J22" s="7"/>
-      <c r="K22" s="7"/>
-      <c r="L22" s="7"/>
-      <c r="M22" s="7"/>
-      <c r="N22" s="7"/>
-      <c r="O22" s="7"/>
-      <c r="P22" s="12"/>
-      <c r="Q22" s="7"/>
-      <c r="R22" s="7"/>
-    </row>
-    <row r="23" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A23" s="16"/>
-      <c r="B23" s="7"/>
-      <c r="C23" s="7"/>
-      <c r="D23" s="7"/>
-      <c r="E23" s="7"/>
-      <c r="F23" s="7"/>
-      <c r="G23" s="7"/>
-      <c r="H23" s="7"/>
-      <c r="I23" s="7"/>
-      <c r="J23" s="7"/>
-      <c r="K23" s="7"/>
-      <c r="L23" s="7"/>
-      <c r="M23" s="7"/>
-      <c r="N23" s="7"/>
-      <c r="O23" s="7"/>
-      <c r="P23" s="12"/>
-      <c r="Q23" s="7"/>
-      <c r="R23" s="7"/>
-    </row>
-    <row r="24" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A24" s="16"/>
-      <c r="B24" s="7"/>
-      <c r="C24" s="7"/>
-      <c r="D24" s="7"/>
-      <c r="E24" s="7"/>
-      <c r="F24" s="7"/>
-      <c r="G24" s="7"/>
-      <c r="H24" s="7"/>
-      <c r="I24" s="7"/>
-      <c r="J24" s="7"/>
-      <c r="K24" s="7"/>
-      <c r="L24" s="7"/>
-      <c r="M24" s="7"/>
-      <c r="N24" s="7"/>
-      <c r="O24" s="7"/>
-      <c r="P24" s="12"/>
-      <c r="Q24" s="7"/>
-      <c r="R24" s="7"/>
-    </row>
-    <row r="25" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A25" s="16"/>
-      <c r="B25" s="7"/>
-      <c r="C25" s="7"/>
-      <c r="D25" s="7"/>
-      <c r="E25" s="7"/>
-      <c r="F25" s="7"/>
-      <c r="G25" s="7"/>
-      <c r="H25" s="7"/>
-      <c r="I25" s="7"/>
-      <c r="J25" s="7"/>
-      <c r="K25" s="7"/>
-      <c r="L25" s="7"/>
-      <c r="M25" s="7"/>
-      <c r="N25" s="7"/>
-      <c r="O25" s="7"/>
-      <c r="P25" s="12"/>
-      <c r="Q25" s="7"/>
-      <c r="R25" s="7"/>
-    </row>
-    <row r="26" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A26" s="16"/>
-      <c r="B26" s="7"/>
-      <c r="C26" s="7"/>
-      <c r="D26" s="7"/>
-      <c r="E26" s="7"/>
-      <c r="F26" s="7"/>
-      <c r="G26" s="7"/>
-      <c r="H26" s="7"/>
-      <c r="I26" s="7"/>
-      <c r="J26" s="7"/>
-      <c r="K26" s="7"/>
-      <c r="L26" s="7"/>
-      <c r="M26" s="7"/>
-      <c r="N26" s="7"/>
-      <c r="O26" s="7"/>
-      <c r="P26" s="12"/>
-      <c r="Q26" s="7"/>
-      <c r="R26" s="7"/>
-    </row>
-    <row r="27" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A27" s="16"/>
-      <c r="B27" s="7"/>
-      <c r="C27" s="7"/>
-      <c r="D27" s="7"/>
-      <c r="E27" s="7"/>
-      <c r="F27" s="7"/>
-      <c r="G27" s="7"/>
-      <c r="H27" s="7"/>
-      <c r="I27" s="7"/>
-      <c r="J27" s="7"/>
-      <c r="K27" s="7"/>
-      <c r="L27" s="7"/>
-      <c r="M27" s="7"/>
-      <c r="N27" s="7"/>
-      <c r="O27" s="7"/>
-      <c r="P27" s="12"/>
-      <c r="Q27" s="7"/>
-      <c r="R27" s="7"/>
-    </row>
-    <row r="28" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A28" s="16"/>
-      <c r="B28" s="7"/>
-      <c r="C28" s="7"/>
-      <c r="D28" s="7"/>
-      <c r="E28" s="7"/>
-      <c r="F28" s="7"/>
-      <c r="G28" s="7"/>
-      <c r="H28" s="7"/>
-      <c r="I28" s="7"/>
-      <c r="J28" s="7"/>
-      <c r="K28" s="7"/>
-      <c r="L28" s="7"/>
-      <c r="M28" s="7"/>
-      <c r="N28" s="7"/>
-      <c r="O28" s="7"/>
-      <c r="P28" s="12"/>
-      <c r="Q28" s="7"/>
-      <c r="R28" s="7"/>
-    </row>
-    <row r="29" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A29" s="16"/>
-      <c r="B29" s="7"/>
-      <c r="C29" s="7"/>
-      <c r="D29" s="7"/>
-      <c r="E29" s="7"/>
-      <c r="F29" s="7"/>
-      <c r="G29" s="7"/>
-      <c r="H29" s="7"/>
-      <c r="I29" s="7"/>
-      <c r="J29" s="7"/>
-      <c r="K29" s="7"/>
-      <c r="L29" s="7"/>
-      <c r="M29" s="7"/>
-      <c r="N29" s="7"/>
-      <c r="O29" s="7"/>
-      <c r="P29" s="12"/>
-      <c r="Q29" s="7"/>
-      <c r="R29" s="7"/>
-    </row>
-    <row r="30" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A30" s="16"/>
-      <c r="B30" s="7"/>
-      <c r="C30" s="7"/>
-      <c r="D30" s="7"/>
-      <c r="E30" s="7"/>
-      <c r="F30" s="7"/>
-      <c r="G30" s="7"/>
-      <c r="H30" s="7"/>
-      <c r="I30" s="7"/>
-      <c r="J30" s="7"/>
-      <c r="K30" s="7"/>
-      <c r="L30" s="7"/>
-      <c r="M30" s="7"/>
-      <c r="N30" s="7"/>
-      <c r="O30" s="7"/>
-      <c r="P30" s="12"/>
-      <c r="Q30" s="7"/>
-      <c r="R30" s="7"/>
-    </row>
-    <row r="31" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A31" s="16"/>
-      <c r="B31" s="7"/>
-      <c r="C31" s="7"/>
-      <c r="D31" s="7"/>
-      <c r="E31" s="7"/>
-      <c r="F31" s="7"/>
-      <c r="G31" s="7"/>
-      <c r="H31" s="7"/>
-      <c r="I31" s="7"/>
-      <c r="J31" s="7"/>
-      <c r="K31" s="7"/>
-      <c r="L31" s="7"/>
-      <c r="M31" s="7"/>
-      <c r="N31" s="7"/>
-      <c r="O31" s="7"/>
-      <c r="P31" s="12"/>
-      <c r="Q31" s="7"/>
-      <c r="R31" s="7"/>
-    </row>
-    <row r="32" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A32" s="16"/>
-      <c r="B32" s="7"/>
-      <c r="C32" s="7"/>
-      <c r="D32" s="7"/>
-      <c r="E32" s="7"/>
-      <c r="F32" s="7"/>
-      <c r="G32" s="7"/>
-      <c r="H32" s="7"/>
-      <c r="I32" s="7"/>
-      <c r="J32" s="7"/>
-      <c r="K32" s="7"/>
-      <c r="L32" s="7"/>
-      <c r="M32" s="7"/>
-      <c r="N32" s="7"/>
-      <c r="O32" s="7"/>
-      <c r="P32" s="12"/>
-      <c r="Q32" s="7"/>
-      <c r="R32" s="7"/>
-    </row>
-    <row r="33" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A33" s="16"/>
-      <c r="B33" s="7"/>
-      <c r="C33" s="7"/>
-      <c r="D33" s="7"/>
-      <c r="E33" s="7"/>
-      <c r="F33" s="7"/>
-      <c r="G33" s="7"/>
-      <c r="H33" s="7"/>
-      <c r="I33" s="7"/>
-      <c r="J33" s="7"/>
-      <c r="K33" s="7"/>
-      <c r="L33" s="7"/>
-      <c r="M33" s="7"/>
-      <c r="N33" s="7"/>
-      <c r="O33" s="7"/>
-      <c r="P33" s="12"/>
-      <c r="Q33" s="7"/>
-      <c r="R33" s="7"/>
-    </row>
-  </sheetData>
-  <mergeCells count="4">
-    <mergeCell ref="F2:G2"/>
-    <mergeCell ref="H2:I2"/>
-    <mergeCell ref="J2:K2"/>
-    <mergeCell ref="P2:R2"/>
-  </mergeCells>
-  <dataValidations count="4">
-    <dataValidation allowBlank="true" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="R5:R33" type="list">
-      <formula1>"PUBLIC,PRIVATE,DISPUTED"</formula1>
-      <formula2>0</formula2>
-    </dataValidation>
-    <dataValidation allowBlank="true" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="F5:K5" type="none">
-      <formula1>0</formula1>
-      <formula2>0</formula2>
-    </dataValidation>
-    <dataValidation allowBlank="true" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="L5:M5" type="none">
-      <formula1>0</formula1>
-      <formula2>0</formula2>
-    </dataValidation>
-    <dataValidation allowBlank="true" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="O5:O33" type="list">
-      <formula1>"Acquisition,Asset,Bridging Loan,Capital,DevelopmentCapital,Growth Finance,Multiple,Program Funding,Property,Property Refurbishment,Other,Restructuring Finance,Startup Costs,Technical Assistance,Unrestricted,Working Capital"</formula1>
       <formula2>0</formula2>
     </dataValidation>
   </dataValidations>
@@ -5365,25 +4598,25 @@
     </row>
     <row r="3" customFormat="false" ht="30" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="17" t="s">
-        <v>423</v>
+        <v>403</v>
       </c>
       <c r="B3" s="17" t="s">
-        <v>381</v>
+        <v>390</v>
       </c>
       <c r="C3" s="17" t="s">
-        <v>424</v>
+        <v>404</v>
       </c>
       <c r="D3" s="4" t="s">
-        <v>425</v>
+        <v>405</v>
       </c>
       <c r="E3" s="10" t="s">
-        <v>426</v>
+        <v>406</v>
       </c>
       <c r="F3" s="10" t="s">
-        <v>427</v>
+        <v>407</v>
       </c>
       <c r="G3" s="10" t="s">
-        <v>428</v>
+        <v>408</v>
       </c>
       <c r="H3" s="4"/>
       <c r="I3" s="4"/>
@@ -5398,7 +4631,7 @@
         <v>15</v>
       </c>
       <c r="N3" s="10" t="s">
-        <v>429</v>
+        <v>409</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="30" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5420,7 +4653,7 @@
         <v>286</v>
       </c>
       <c r="J4" s="10" t="s">
-        <v>400</v>
+        <v>410</v>
       </c>
       <c r="K4" s="11"/>
       <c r="L4" s="4"/>
@@ -5429,46 +4662,46 @@
     </row>
     <row r="5" customFormat="false" ht="115.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="12" t="s">
-        <v>430</v>
+        <v>411</v>
       </c>
       <c r="B5" s="12" t="s">
-        <v>431</v>
+        <v>412</v>
       </c>
       <c r="C5" s="12" t="s">
-        <v>432</v>
+        <v>413</v>
       </c>
       <c r="D5" s="7" t="s">
-        <v>433</v>
+        <v>414</v>
       </c>
       <c r="E5" s="7" t="s">
-        <v>434</v>
+        <v>415</v>
       </c>
       <c r="F5" s="7" t="s">
-        <v>435</v>
+        <v>416</v>
       </c>
       <c r="G5" s="7" t="s">
-        <v>436</v>
+        <v>417</v>
       </c>
       <c r="H5" s="7" t="s">
-        <v>437</v>
+        <v>418</v>
       </c>
       <c r="I5" s="7" t="s">
-        <v>438</v>
+        <v>419</v>
       </c>
       <c r="J5" s="7" t="s">
-        <v>439</v>
+        <v>420</v>
       </c>
       <c r="K5" s="12" t="s">
-        <v>440</v>
+        <v>421</v>
       </c>
       <c r="L5" s="7" t="s">
-        <v>441</v>
+        <v>422</v>
       </c>
       <c r="M5" s="7" t="s">
-        <v>442</v>
+        <v>423</v>
       </c>
       <c r="N5" s="7" t="s">
-        <v>443</v>
+        <v>424</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5993,22 +5226,22 @@
         <v>263</v>
       </c>
       <c r="B3" s="10" t="s">
-        <v>398</v>
+        <v>425</v>
       </c>
       <c r="C3" s="10" t="s">
         <v>268</v>
       </c>
       <c r="D3" s="10" t="s">
-        <v>444</v>
+        <v>426</v>
       </c>
       <c r="E3" s="10" t="s">
-        <v>445</v>
+        <v>427</v>
       </c>
       <c r="F3" s="10" t="s">
-        <v>446</v>
+        <v>428</v>
       </c>
       <c r="G3" s="10" t="s">
-        <v>447</v>
+        <v>429</v>
       </c>
       <c r="H3" s="10" t="s">
         <v>285</v>
@@ -6028,10 +5261,10 @@
       <c r="B4" s="10"/>
       <c r="C4" s="10"/>
       <c r="D4" s="10" t="s">
-        <v>404</v>
+        <v>430</v>
       </c>
       <c r="E4" s="10" t="s">
-        <v>404</v>
+        <v>430</v>
       </c>
       <c r="F4" s="10"/>
       <c r="G4" s="10"/>
@@ -6042,37 +5275,37 @@
     </row>
     <row r="5" customFormat="false" ht="114.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="16" t="s">
-        <v>448</v>
+        <v>431</v>
       </c>
       <c r="B5" s="7" t="s">
-        <v>449</v>
+        <v>432</v>
       </c>
       <c r="C5" s="7" t="s">
-        <v>450</v>
+        <v>433</v>
       </c>
       <c r="D5" s="7" t="s">
-        <v>451</v>
+        <v>434</v>
       </c>
       <c r="E5" s="7" t="s">
-        <v>452</v>
+        <v>435</v>
       </c>
       <c r="F5" s="7" t="s">
-        <v>453</v>
+        <v>436</v>
       </c>
       <c r="G5" s="7" t="s">
-        <v>454</v>
+        <v>437</v>
       </c>
       <c r="H5" s="7" t="s">
-        <v>455</v>
+        <v>438</v>
       </c>
       <c r="I5" s="12" t="s">
-        <v>456</v>
+        <v>439</v>
       </c>
       <c r="J5" s="7" t="s">
-        <v>457</v>
+        <v>440</v>
       </c>
       <c r="K5" s="7" t="s">
-        <v>458</v>
+        <v>441</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6515,29 +5748,29 @@
     </row>
     <row r="3" customFormat="false" ht="44" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A3" s="17" t="s">
-        <v>459</v>
+        <v>442</v>
       </c>
       <c r="B3" s="4" t="s">
-        <v>398</v>
+        <v>425</v>
       </c>
       <c r="C3" s="4" t="s">
         <v>268</v>
       </c>
       <c r="D3" s="4" t="s">
-        <v>460</v>
+        <v>443</v>
       </c>
       <c r="E3" s="4" t="s">
-        <v>461</v>
+        <v>444</v>
       </c>
       <c r="F3" s="4" t="s">
-        <v>462</v>
+        <v>445</v>
       </c>
       <c r="G3" s="10" t="s">
-        <v>463</v>
+        <v>446</v>
       </c>
       <c r="H3" s="10"/>
       <c r="I3" s="10" t="s">
-        <v>464</v>
+        <v>447</v>
       </c>
       <c r="J3" s="11" t="s">
         <v>189</v>
@@ -6560,7 +5793,7 @@
         <v>286</v>
       </c>
       <c r="H4" s="10" t="s">
-        <v>400</v>
+        <v>410</v>
       </c>
       <c r="I4" s="4"/>
       <c r="J4" s="11"/>
@@ -6569,40 +5802,40 @@
     </row>
     <row r="5" customFormat="false" ht="129.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="12" t="s">
-        <v>465</v>
+        <v>448</v>
       </c>
       <c r="B5" s="7" t="s">
-        <v>466</v>
+        <v>449</v>
       </c>
       <c r="C5" s="7" t="s">
-        <v>467</v>
+        <v>450</v>
       </c>
       <c r="D5" s="7" t="s">
-        <v>468</v>
+        <v>451</v>
       </c>
       <c r="E5" s="7" t="s">
-        <v>469</v>
+        <v>452</v>
       </c>
       <c r="F5" s="7" t="s">
-        <v>470</v>
+        <v>453</v>
       </c>
       <c r="G5" s="7" t="s">
-        <v>471</v>
+        <v>454</v>
       </c>
       <c r="H5" s="7" t="s">
-        <v>472</v>
+        <v>455</v>
       </c>
       <c r="I5" s="7" t="s">
-        <v>473</v>
+        <v>456</v>
       </c>
       <c r="J5" s="12" t="s">
-        <v>474</v>
+        <v>457</v>
       </c>
       <c r="K5" s="7" t="s">
-        <v>475</v>
+        <v>458</v>
       </c>
       <c r="L5" s="7" t="s">
-        <v>476</v>
+        <v>459</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7061,277 +6294,277 @@
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="0" t="s">
-        <v>477</v>
+        <v>460</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="0" t="s">
-        <v>478</v>
+        <v>461</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="0" t="s">
-        <v>479</v>
+        <v>462</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="0" t="s">
-        <v>480</v>
+        <v>463</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="0" t="s">
-        <v>481</v>
+        <v>464</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="0" t="s">
-        <v>482</v>
+        <v>465</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="0" t="s">
-        <v>483</v>
+        <v>466</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="0" t="s">
-        <v>484</v>
+        <v>467</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="0" t="s">
-        <v>485</v>
+        <v>468</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="0" t="s">
-        <v>486</v>
+        <v>469</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="0" t="s">
-        <v>487</v>
+        <v>470</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="0" t="s">
-        <v>488</v>
+        <v>471</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="0" t="s">
-        <v>489</v>
+        <v>472</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="0" t="s">
-        <v>490</v>
+        <v>473</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="0" t="s">
-        <v>491</v>
+        <v>474</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="0" t="s">
-        <v>492</v>
+        <v>475</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="0" t="s">
-        <v>493</v>
+        <v>476</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="0" t="s">
-        <v>494</v>
+        <v>477</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="0" t="s">
-        <v>495</v>
+        <v>478</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="0" t="s">
-        <v>496</v>
+        <v>479</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="0" t="s">
-        <v>497</v>
+        <v>480</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="0" t="s">
-        <v>498</v>
+        <v>481</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="0" t="s">
-        <v>499</v>
+        <v>482</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A26" s="0" t="s">
-        <v>500</v>
+        <v>483</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A27" s="0" t="s">
-        <v>501</v>
+        <v>484</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A28" s="0" t="s">
-        <v>502</v>
+        <v>485</v>
       </c>
     </row>
     <row r="29" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A29" s="0" t="s">
-        <v>503</v>
+        <v>486</v>
       </c>
     </row>
     <row r="30" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A30" s="0" t="s">
-        <v>504</v>
+        <v>487</v>
       </c>
     </row>
     <row r="31" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A31" s="0" t="s">
-        <v>505</v>
+        <v>488</v>
       </c>
     </row>
     <row r="32" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A32" s="0" t="s">
-        <v>506</v>
+        <v>489</v>
       </c>
     </row>
     <row r="33" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A33" s="0" t="s">
-        <v>507</v>
+        <v>490</v>
       </c>
     </row>
     <row r="34" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A34" s="0" t="s">
-        <v>508</v>
+        <v>491</v>
       </c>
     </row>
     <row r="35" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A35" s="0" t="s">
-        <v>509</v>
+        <v>492</v>
       </c>
     </row>
     <row r="36" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A36" s="0" t="s">
-        <v>510</v>
+        <v>493</v>
       </c>
     </row>
     <row r="37" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A37" s="0" t="s">
-        <v>511</v>
+        <v>494</v>
       </c>
     </row>
     <row r="38" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A38" s="0" t="s">
-        <v>512</v>
+        <v>495</v>
       </c>
     </row>
     <row r="39" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A39" s="0" t="s">
-        <v>513</v>
+        <v>496</v>
       </c>
     </row>
     <row r="40" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A40" s="0" t="s">
-        <v>514</v>
+        <v>497</v>
       </c>
     </row>
     <row r="41" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A41" s="0" t="s">
-        <v>515</v>
+        <v>498</v>
       </c>
     </row>
     <row r="42" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A42" s="0" t="s">
-        <v>516</v>
+        <v>499</v>
       </c>
     </row>
     <row r="43" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A43" s="0" t="s">
-        <v>517</v>
+        <v>500</v>
       </c>
     </row>
     <row r="44" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A44" s="0" t="s">
-        <v>518</v>
+        <v>501</v>
       </c>
     </row>
     <row r="45" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A45" s="0" t="s">
-        <v>519</v>
+        <v>502</v>
       </c>
     </row>
     <row r="46" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A46" s="0" t="s">
-        <v>520</v>
+        <v>503</v>
       </c>
     </row>
     <row r="47" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A47" s="0" t="s">
-        <v>521</v>
+        <v>504</v>
       </c>
     </row>
     <row r="48" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A48" s="0" t="s">
-        <v>522</v>
+        <v>505</v>
       </c>
     </row>
     <row r="49" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A49" s="0" t="s">
-        <v>523</v>
+        <v>506</v>
       </c>
     </row>
     <row r="50" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A50" s="0" t="s">
-        <v>524</v>
+        <v>507</v>
       </c>
     </row>
     <row r="51" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A51" s="0" t="s">
-        <v>525</v>
+        <v>508</v>
       </c>
     </row>
     <row r="52" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A52" s="0" t="s">
-        <v>526</v>
+        <v>509</v>
       </c>
     </row>
     <row r="53" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A53" s="0" t="s">
-        <v>527</v>
+        <v>510</v>
       </c>
     </row>
     <row r="54" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A54" s="0" t="s">
-        <v>528</v>
+        <v>511</v>
       </c>
     </row>
     <row r="55" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A55" s="0" t="s">
-        <v>529</v>
+        <v>512</v>
       </c>
     </row>
     <row r="56" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A56" s="0" t="s">
-        <v>530</v>
+        <v>513</v>
       </c>
     </row>
     <row r="57" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A57" s="0" t="s">
-        <v>531</v>
+        <v>514</v>
       </c>
     </row>
   </sheetData>
@@ -7396,10 +6629,10 @@
     </row>
     <row r="3" customFormat="false" ht="30" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="17" t="s">
-        <v>381</v>
+        <v>390</v>
       </c>
       <c r="B3" s="4" t="s">
-        <v>532</v>
+        <v>515</v>
       </c>
       <c r="C3" s="4" t="s">
         <v>288</v>
@@ -7411,22 +6644,22 @@
         <v>290</v>
       </c>
       <c r="F3" s="4" t="s">
-        <v>533</v>
+        <v>516</v>
       </c>
       <c r="G3" s="10" t="s">
-        <v>534</v>
+        <v>517</v>
       </c>
       <c r="H3" s="10" t="s">
-        <v>535</v>
+        <v>518</v>
       </c>
       <c r="I3" s="10" t="s">
-        <v>536</v>
+        <v>519</v>
       </c>
       <c r="J3" s="11" t="s">
-        <v>537</v>
+        <v>520</v>
       </c>
       <c r="K3" s="11" t="s">
-        <v>538</v>
+        <v>521</v>
       </c>
       <c r="L3" s="11" t="s">
         <v>189</v>
@@ -7449,10 +6682,10 @@
       <c r="H4" s="4"/>
       <c r="I4" s="4"/>
       <c r="J4" s="11" t="s">
-        <v>539</v>
+        <v>522</v>
       </c>
       <c r="K4" s="11" t="s">
-        <v>540</v>
+        <v>523</v>
       </c>
       <c r="L4" s="11"/>
       <c r="M4" s="4"/>
@@ -7460,46 +6693,46 @@
     </row>
     <row r="5" customFormat="false" ht="72.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="12" t="s">
-        <v>541</v>
+        <v>524</v>
       </c>
       <c r="B5" s="7" t="s">
-        <v>542</v>
+        <v>525</v>
       </c>
       <c r="C5" s="7" t="s">
-        <v>543</v>
+        <v>526</v>
       </c>
       <c r="D5" s="7" t="s">
-        <v>544</v>
+        <v>527</v>
       </c>
       <c r="E5" s="7" t="s">
-        <v>545</v>
+        <v>528</v>
       </c>
       <c r="F5" s="7" t="s">
-        <v>546</v>
+        <v>529</v>
       </c>
       <c r="G5" s="7" t="s">
-        <v>547</v>
+        <v>530</v>
       </c>
       <c r="H5" s="7" t="s">
-        <v>548</v>
+        <v>531</v>
       </c>
       <c r="I5" s="7" t="s">
-        <v>549</v>
+        <v>532</v>
       </c>
       <c r="J5" s="12" t="s">
-        <v>550</v>
+        <v>533</v>
       </c>
       <c r="K5" s="12" t="s">
-        <v>551</v>
+        <v>534</v>
       </c>
       <c r="L5" s="12" t="s">
-        <v>552</v>
+        <v>535</v>
       </c>
       <c r="M5" s="7" t="s">
-        <v>553</v>
+        <v>536</v>
       </c>
       <c r="N5" s="7" t="s">
-        <v>554</v>
+        <v>537</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -8023,7 +7256,7 @@
     </row>
     <row r="3" customFormat="false" ht="44.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="17" t="s">
-        <v>381</v>
+        <v>390</v>
       </c>
       <c r="B3" s="4" t="s">
         <v>289</v>
@@ -8032,16 +7265,16 @@
         <v>290</v>
       </c>
       <c r="D3" s="17" t="s">
-        <v>555</v>
+        <v>538</v>
       </c>
       <c r="E3" s="17" t="s">
-        <v>556</v>
+        <v>539</v>
       </c>
       <c r="F3" s="10" t="s">
-        <v>557</v>
+        <v>540</v>
       </c>
       <c r="G3" s="4" t="s">
-        <v>558</v>
+        <v>541</v>
       </c>
       <c r="H3" s="4"/>
       <c r="I3" s="4"/>
@@ -8055,7 +7288,7 @@
         <v>15</v>
       </c>
       <c r="M3" s="10" t="s">
-        <v>429</v>
+        <v>409</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="30" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -8076,7 +7309,7 @@
         <v>286</v>
       </c>
       <c r="I4" s="10" t="s">
-        <v>400</v>
+        <v>410</v>
       </c>
       <c r="J4" s="11"/>
       <c r="K4" s="4"/>
@@ -8085,43 +7318,43 @@
     </row>
     <row r="5" customFormat="false" ht="129.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="12" t="s">
-        <v>559</v>
+        <v>542</v>
       </c>
       <c r="B5" s="7" t="s">
-        <v>560</v>
+        <v>543</v>
       </c>
       <c r="C5" s="7" t="s">
-        <v>561</v>
+        <v>544</v>
       </c>
       <c r="D5" s="12" t="s">
-        <v>562</v>
+        <v>545</v>
       </c>
       <c r="E5" s="12" t="s">
-        <v>563</v>
+        <v>546</v>
       </c>
       <c r="F5" s="7" t="s">
-        <v>564</v>
+        <v>547</v>
       </c>
       <c r="G5" s="7" t="s">
-        <v>565</v>
+        <v>548</v>
       </c>
       <c r="H5" s="7" t="s">
-        <v>566</v>
+        <v>549</v>
       </c>
       <c r="I5" s="7" t="s">
-        <v>567</v>
+        <v>550</v>
       </c>
       <c r="J5" s="12" t="s">
-        <v>568</v>
+        <v>551</v>
       </c>
       <c r="K5" s="7" t="s">
-        <v>569</v>
+        <v>552</v>
       </c>
       <c r="L5" s="7" t="s">
-        <v>570</v>
+        <v>553</v>
       </c>
       <c r="M5" s="7" t="s">
-        <v>571</v>
+        <v>554</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -8633,8 +7866,8 @@
   </sheetPr>
   <dimension ref="A2:F87"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A44" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="C51" activeCellId="0" sqref="C51"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -9665,7 +8898,7 @@
     </row>
     <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="4" t="s">
-        <v>572</v>
+        <v>555</v>
       </c>
       <c r="B3" s="11" t="s">
         <v>189</v>
@@ -9679,16 +8912,16 @@
     </row>
     <row r="4" customFormat="false" ht="101.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="7" t="s">
-        <v>573</v>
+        <v>556</v>
       </c>
       <c r="B4" s="12" t="s">
-        <v>574</v>
+        <v>557</v>
       </c>
       <c r="C4" s="7" t="s">
-        <v>575</v>
+        <v>558</v>
       </c>
       <c r="D4" s="7" t="s">
-        <v>576</v>
+        <v>559</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -9905,7 +9138,7 @@
     </row>
     <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="4" t="s">
-        <v>424</v>
+        <v>404</v>
       </c>
       <c r="B3" s="11" t="s">
         <v>189</v>
@@ -9919,16 +9152,16 @@
     </row>
     <row r="4" customFormat="false" ht="87" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="7" t="s">
-        <v>577</v>
+        <v>560</v>
       </c>
       <c r="B4" s="12" t="s">
-        <v>578</v>
+        <v>561</v>
       </c>
       <c r="C4" s="7" t="s">
-        <v>579</v>
+        <v>562</v>
       </c>
       <c r="D4" s="7" t="s">
-        <v>580</v>
+        <v>563</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -10147,7 +9380,7 @@
     </row>
     <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="4" t="s">
-        <v>398</v>
+        <v>425</v>
       </c>
       <c r="B3" s="4" t="s">
         <v>224</v>
@@ -10161,16 +9394,16 @@
     </row>
     <row r="4" customFormat="false" ht="72.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="7" t="s">
-        <v>581</v>
+        <v>564</v>
       </c>
       <c r="B4" s="7" t="s">
-        <v>582</v>
+        <v>565</v>
       </c>
       <c r="C4" s="7" t="s">
-        <v>583</v>
+        <v>566</v>
       </c>
       <c r="D4" s="7" t="s">
-        <v>584</v>
+        <v>567</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -10380,502 +9613,502 @@
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="0" t="s">
-        <v>585</v>
+        <v>568</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="s">
-        <v>586</v>
+        <v>569</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="s">
-        <v>587</v>
+        <v>570</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="0" t="s">
-        <v>588</v>
+        <v>571</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="0" t="s">
-        <v>589</v>
+        <v>572</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="0" t="s">
-        <v>590</v>
+        <v>573</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="0" t="s">
-        <v>591</v>
+        <v>574</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="0" t="s">
-        <v>592</v>
+        <v>575</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="0" t="s">
-        <v>593</v>
+        <v>576</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="0" t="s">
-        <v>594</v>
+        <v>577</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="0" t="s">
-        <v>595</v>
+        <v>578</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="0" t="s">
-        <v>596</v>
+        <v>579</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="0" t="s">
-        <v>597</v>
+        <v>580</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="0" t="s">
-        <v>598</v>
+        <v>581</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="0" t="s">
-        <v>599</v>
+        <v>582</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="0" t="s">
-        <v>600</v>
+        <v>583</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="0" t="s">
-        <v>601</v>
+        <v>584</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="0" t="s">
-        <v>602</v>
+        <v>585</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="0" t="s">
-        <v>603</v>
+        <v>586</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="0" t="s">
-        <v>604</v>
+        <v>587</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="0" t="s">
-        <v>605</v>
+        <v>588</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="0" t="s">
-        <v>606</v>
+        <v>589</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="0" t="s">
-        <v>607</v>
+        <v>590</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="0" t="s">
-        <v>608</v>
+        <v>591</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="0" t="s">
-        <v>609</v>
+        <v>592</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A26" s="0" t="s">
-        <v>610</v>
+        <v>593</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A27" s="0" t="s">
-        <v>611</v>
+        <v>594</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A28" s="0" t="s">
-        <v>612</v>
+        <v>595</v>
       </c>
     </row>
     <row r="29" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A29" s="0" t="s">
-        <v>613</v>
+        <v>596</v>
       </c>
     </row>
     <row r="30" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A30" s="0" t="s">
-        <v>614</v>
+        <v>597</v>
       </c>
     </row>
     <row r="31" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A31" s="0" t="s">
-        <v>615</v>
+        <v>598</v>
       </c>
     </row>
     <row r="32" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A32" s="0" t="s">
-        <v>616</v>
+        <v>599</v>
       </c>
     </row>
     <row r="33" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A33" s="0" t="s">
-        <v>617</v>
+        <v>600</v>
       </c>
     </row>
     <row r="34" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A34" s="0" t="s">
-        <v>618</v>
+        <v>601</v>
       </c>
     </row>
     <row r="35" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A35" s="0" t="s">
-        <v>619</v>
+        <v>602</v>
       </c>
     </row>
     <row r="36" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A36" s="0" t="s">
-        <v>620</v>
+        <v>603</v>
       </c>
     </row>
     <row r="37" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A37" s="0" t="s">
-        <v>621</v>
+        <v>604</v>
       </c>
     </row>
     <row r="38" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A38" s="0" t="s">
-        <v>622</v>
+        <v>605</v>
       </c>
     </row>
     <row r="39" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A39" s="0" t="s">
-        <v>623</v>
+        <v>606</v>
       </c>
     </row>
     <row r="40" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A40" s="0" t="s">
-        <v>624</v>
+        <v>607</v>
       </c>
     </row>
     <row r="41" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A41" s="0" t="s">
-        <v>625</v>
+        <v>608</v>
       </c>
     </row>
     <row r="42" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A42" s="0" t="s">
-        <v>626</v>
+        <v>609</v>
       </c>
     </row>
     <row r="43" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A43" s="0" t="s">
-        <v>627</v>
+        <v>610</v>
       </c>
     </row>
     <row r="44" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A44" s="0" t="s">
-        <v>628</v>
+        <v>611</v>
       </c>
     </row>
     <row r="45" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A45" s="0" t="s">
-        <v>629</v>
+        <v>612</v>
       </c>
     </row>
     <row r="46" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A46" s="0" t="s">
-        <v>630</v>
+        <v>613</v>
       </c>
     </row>
     <row r="47" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A47" s="0" t="s">
-        <v>631</v>
+        <v>614</v>
       </c>
     </row>
     <row r="48" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A48" s="0" t="s">
-        <v>632</v>
+        <v>615</v>
       </c>
     </row>
     <row r="49" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A49" s="0" t="s">
-        <v>633</v>
+        <v>616</v>
       </c>
     </row>
     <row r="50" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A50" s="0" t="s">
-        <v>634</v>
+        <v>617</v>
       </c>
     </row>
     <row r="51" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A51" s="0" t="s">
-        <v>635</v>
+        <v>618</v>
       </c>
     </row>
     <row r="52" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A52" s="0" t="s">
-        <v>636</v>
+        <v>619</v>
       </c>
     </row>
     <row r="53" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A53" s="0" t="s">
-        <v>637</v>
+        <v>620</v>
       </c>
     </row>
     <row r="54" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A54" s="0" t="s">
-        <v>638</v>
+        <v>621</v>
       </c>
     </row>
     <row r="55" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A55" s="0" t="s">
-        <v>639</v>
+        <v>622</v>
       </c>
     </row>
     <row r="56" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A56" s="0" t="s">
-        <v>640</v>
+        <v>623</v>
       </c>
     </row>
     <row r="57" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A57" s="0" t="s">
-        <v>641</v>
+        <v>624</v>
       </c>
     </row>
     <row r="58" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A58" s="0" t="s">
-        <v>642</v>
+        <v>625</v>
       </c>
     </row>
     <row r="59" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A59" s="0" t="s">
-        <v>643</v>
+        <v>626</v>
       </c>
     </row>
     <row r="60" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A60" s="0" t="s">
-        <v>644</v>
+        <v>627</v>
       </c>
     </row>
     <row r="61" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A61" s="0" t="s">
-        <v>645</v>
+        <v>628</v>
       </c>
     </row>
     <row r="62" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A62" s="0" t="s">
-        <v>646</v>
+        <v>629</v>
       </c>
     </row>
     <row r="63" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A63" s="0" t="s">
-        <v>647</v>
+        <v>630</v>
       </c>
     </row>
     <row r="64" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A64" s="0" t="s">
-        <v>648</v>
+        <v>631</v>
       </c>
     </row>
     <row r="65" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A65" s="0" t="s">
-        <v>649</v>
+        <v>632</v>
       </c>
     </row>
     <row r="66" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A66" s="0" t="s">
-        <v>650</v>
+        <v>633</v>
       </c>
     </row>
     <row r="67" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A67" s="0" t="s">
-        <v>651</v>
+        <v>634</v>
       </c>
     </row>
     <row r="68" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A68" s="0" t="s">
-        <v>652</v>
+        <v>635</v>
       </c>
     </row>
     <row r="69" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A69" s="0" t="s">
-        <v>653</v>
+        <v>636</v>
       </c>
     </row>
     <row r="70" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A70" s="0" t="s">
-        <v>654</v>
+        <v>637</v>
       </c>
     </row>
     <row r="71" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A71" s="0" t="s">
-        <v>655</v>
+        <v>638</v>
       </c>
     </row>
     <row r="72" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A72" s="0" t="s">
-        <v>656</v>
+        <v>639</v>
       </c>
     </row>
     <row r="73" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A73" s="0" t="s">
-        <v>657</v>
+        <v>640</v>
       </c>
     </row>
     <row r="74" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A74" s="0" t="s">
-        <v>658</v>
+        <v>641</v>
       </c>
     </row>
     <row r="75" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A75" s="0" t="s">
-        <v>659</v>
+        <v>642</v>
       </c>
     </row>
     <row r="76" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A76" s="0" t="s">
-        <v>660</v>
+        <v>643</v>
       </c>
     </row>
     <row r="77" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A77" s="0" t="s">
-        <v>661</v>
+        <v>644</v>
       </c>
     </row>
     <row r="78" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A78" s="0" t="s">
-        <v>662</v>
+        <v>645</v>
       </c>
     </row>
     <row r="79" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A79" s="0" t="s">
-        <v>663</v>
+        <v>646</v>
       </c>
     </row>
     <row r="80" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A80" s="0" t="s">
-        <v>664</v>
+        <v>647</v>
       </c>
     </row>
     <row r="81" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A81" s="0" t="s">
-        <v>665</v>
+        <v>648</v>
       </c>
     </row>
     <row r="82" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A82" s="0" t="s">
-        <v>666</v>
+        <v>649</v>
       </c>
     </row>
     <row r="83" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A83" s="0" t="s">
-        <v>667</v>
+        <v>650</v>
       </c>
     </row>
     <row r="84" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A84" s="0" t="s">
-        <v>668</v>
+        <v>651</v>
       </c>
     </row>
     <row r="85" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A85" s="0" t="s">
-        <v>669</v>
+        <v>652</v>
       </c>
     </row>
     <row r="86" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A86" s="0" t="s">
-        <v>670</v>
+        <v>653</v>
       </c>
     </row>
     <row r="87" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A87" s="0" t="s">
-        <v>671</v>
+        <v>654</v>
       </c>
     </row>
     <row r="88" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A88" s="0" t="s">
-        <v>672</v>
+        <v>655</v>
       </c>
     </row>
     <row r="89" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A89" s="0" t="s">
-        <v>673</v>
+        <v>656</v>
       </c>
     </row>
     <row r="90" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A90" s="0" t="s">
-        <v>674</v>
+        <v>657</v>
       </c>
     </row>
     <row r="91" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A91" s="0" t="s">
-        <v>675</v>
+        <v>658</v>
       </c>
     </row>
     <row r="92" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A92" s="0" t="s">
-        <v>676</v>
+        <v>659</v>
       </c>
     </row>
     <row r="93" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A93" s="0" t="s">
-        <v>677</v>
+        <v>660</v>
       </c>
     </row>
     <row r="94" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A94" s="0" t="s">
-        <v>678</v>
+        <v>661</v>
       </c>
     </row>
     <row r="95" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A95" s="0" t="s">
-        <v>679</v>
+        <v>662</v>
       </c>
     </row>
     <row r="96" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A96" s="0" t="s">
-        <v>680</v>
+        <v>663</v>
       </c>
     </row>
     <row r="97" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A97" s="0" t="s">
-        <v>681</v>
+        <v>664</v>
       </c>
     </row>
     <row r="98" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A98" s="0" t="s">
-        <v>682</v>
+        <v>665</v>
       </c>
     </row>
     <row r="99" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A99" s="0" t="s">
-        <v>683</v>
+        <v>666</v>
       </c>
     </row>
     <row r="100" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A100" s="0" t="s">
-        <v>684</v>
+        <v>667</v>
       </c>
     </row>
     <row r="101" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -10885,742 +10118,742 @@
     </row>
     <row r="102" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A102" s="0" t="s">
-        <v>685</v>
+        <v>668</v>
       </c>
     </row>
     <row r="103" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A103" s="0" t="s">
-        <v>686</v>
+        <v>669</v>
       </c>
     </row>
     <row r="104" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A104" s="0" t="s">
-        <v>687</v>
+        <v>670</v>
       </c>
     </row>
     <row r="105" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A105" s="0" t="s">
-        <v>688</v>
+        <v>671</v>
       </c>
     </row>
     <row r="106" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A106" s="0" t="s">
-        <v>689</v>
+        <v>672</v>
       </c>
     </row>
     <row r="107" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A107" s="0" t="s">
-        <v>690</v>
+        <v>673</v>
       </c>
     </row>
     <row r="108" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A108" s="0" t="s">
-        <v>691</v>
+        <v>674</v>
       </c>
     </row>
     <row r="109" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A109" s="0" t="s">
-        <v>692</v>
+        <v>675</v>
       </c>
     </row>
     <row r="110" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A110" s="0" t="s">
-        <v>693</v>
+        <v>676</v>
       </c>
     </row>
     <row r="111" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A111" s="0" t="s">
-        <v>694</v>
+        <v>677</v>
       </c>
     </row>
     <row r="112" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A112" s="0" t="s">
-        <v>695</v>
+        <v>678</v>
       </c>
     </row>
     <row r="113" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A113" s="0" t="s">
-        <v>696</v>
+        <v>679</v>
       </c>
     </row>
     <row r="114" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A114" s="0" t="s">
-        <v>697</v>
+        <v>680</v>
       </c>
     </row>
     <row r="115" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A115" s="0" t="s">
-        <v>698</v>
+        <v>681</v>
       </c>
     </row>
     <row r="116" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A116" s="0" t="s">
-        <v>699</v>
+        <v>682</v>
       </c>
     </row>
     <row r="117" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A117" s="0" t="s">
-        <v>700</v>
+        <v>683</v>
       </c>
     </row>
     <row r="118" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A118" s="0" t="s">
-        <v>701</v>
+        <v>684</v>
       </c>
     </row>
     <row r="119" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A119" s="0" t="s">
-        <v>702</v>
+        <v>685</v>
       </c>
     </row>
     <row r="120" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A120" s="0" t="s">
-        <v>703</v>
+        <v>686</v>
       </c>
     </row>
     <row r="121" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A121" s="0" t="s">
-        <v>704</v>
+        <v>687</v>
       </c>
     </row>
     <row r="122" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A122" s="0" t="s">
-        <v>705</v>
+        <v>688</v>
       </c>
     </row>
     <row r="123" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A123" s="0" t="s">
-        <v>706</v>
+        <v>689</v>
       </c>
     </row>
     <row r="124" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A124" s="0" t="s">
-        <v>707</v>
+        <v>690</v>
       </c>
     </row>
     <row r="125" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A125" s="0" t="s">
-        <v>708</v>
+        <v>691</v>
       </c>
     </row>
     <row r="126" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A126" s="0" t="s">
-        <v>709</v>
+        <v>692</v>
       </c>
     </row>
     <row r="127" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A127" s="0" t="s">
-        <v>710</v>
+        <v>693</v>
       </c>
     </row>
     <row r="128" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A128" s="0" t="s">
-        <v>711</v>
+        <v>694</v>
       </c>
     </row>
     <row r="129" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A129" s="0" t="s">
-        <v>712</v>
+        <v>695</v>
       </c>
     </row>
     <row r="130" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A130" s="0" t="s">
-        <v>713</v>
+        <v>696</v>
       </c>
     </row>
     <row r="131" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A131" s="0" t="s">
-        <v>714</v>
+        <v>697</v>
       </c>
     </row>
     <row r="132" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A132" s="0" t="s">
-        <v>715</v>
+        <v>698</v>
       </c>
     </row>
     <row r="133" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A133" s="0" t="s">
-        <v>716</v>
+        <v>699</v>
       </c>
     </row>
     <row r="134" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A134" s="0" t="s">
-        <v>717</v>
+        <v>700</v>
       </c>
     </row>
     <row r="135" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A135" s="0" t="s">
-        <v>718</v>
+        <v>701</v>
       </c>
     </row>
     <row r="136" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A136" s="0" t="s">
-        <v>719</v>
+        <v>702</v>
       </c>
     </row>
     <row r="137" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A137" s="0" t="s">
-        <v>720</v>
+        <v>703</v>
       </c>
     </row>
     <row r="138" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A138" s="0" t="s">
-        <v>721</v>
+        <v>704</v>
       </c>
     </row>
     <row r="139" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A139" s="0" t="s">
-        <v>722</v>
+        <v>705</v>
       </c>
     </row>
     <row r="140" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A140" s="0" t="s">
-        <v>723</v>
+        <v>706</v>
       </c>
     </row>
     <row r="141" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A141" s="0" t="s">
-        <v>724</v>
+        <v>707</v>
       </c>
     </row>
     <row r="142" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A142" s="0" t="s">
-        <v>725</v>
+        <v>708</v>
       </c>
     </row>
     <row r="143" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A143" s="0" t="s">
-        <v>726</v>
+        <v>709</v>
       </c>
     </row>
     <row r="144" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A144" s="0" t="s">
-        <v>727</v>
+        <v>710</v>
       </c>
     </row>
     <row r="145" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A145" s="0" t="s">
-        <v>728</v>
+        <v>711</v>
       </c>
     </row>
     <row r="146" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A146" s="0" t="s">
-        <v>729</v>
+        <v>712</v>
       </c>
     </row>
     <row r="147" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A147" s="0" t="s">
-        <v>730</v>
+        <v>713</v>
       </c>
     </row>
     <row r="148" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A148" s="0" t="s">
-        <v>731</v>
+        <v>714</v>
       </c>
     </row>
     <row r="149" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A149" s="0" t="s">
-        <v>732</v>
+        <v>715</v>
       </c>
     </row>
     <row r="150" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A150" s="0" t="s">
-        <v>733</v>
+        <v>716</v>
       </c>
     </row>
     <row r="151" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A151" s="0" t="s">
-        <v>734</v>
+        <v>717</v>
       </c>
     </row>
     <row r="152" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A152" s="0" t="s">
-        <v>735</v>
+        <v>718</v>
       </c>
     </row>
     <row r="153" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A153" s="0" t="s">
-        <v>736</v>
+        <v>719</v>
       </c>
     </row>
     <row r="154" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A154" s="0" t="s">
-        <v>737</v>
+        <v>720</v>
       </c>
     </row>
     <row r="155" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A155" s="0" t="s">
-        <v>738</v>
+        <v>721</v>
       </c>
     </row>
     <row r="156" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A156" s="0" t="s">
-        <v>739</v>
+        <v>722</v>
       </c>
     </row>
     <row r="157" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A157" s="0" t="s">
-        <v>740</v>
+        <v>723</v>
       </c>
     </row>
     <row r="158" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A158" s="0" t="s">
-        <v>741</v>
+        <v>724</v>
       </c>
     </row>
     <row r="159" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A159" s="0" t="s">
-        <v>742</v>
+        <v>725</v>
       </c>
     </row>
     <row r="160" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A160" s="0" t="s">
-        <v>743</v>
+        <v>726</v>
       </c>
     </row>
     <row r="161" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A161" s="0" t="s">
-        <v>744</v>
+        <v>727</v>
       </c>
     </row>
     <row r="162" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A162" s="0" t="s">
-        <v>745</v>
+        <v>728</v>
       </c>
     </row>
     <row r="163" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A163" s="0" t="s">
-        <v>746</v>
+        <v>729</v>
       </c>
     </row>
     <row r="164" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A164" s="0" t="s">
-        <v>747</v>
+        <v>730</v>
       </c>
     </row>
     <row r="165" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A165" s="0" t="s">
-        <v>748</v>
+        <v>731</v>
       </c>
     </row>
     <row r="166" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A166" s="0" t="s">
-        <v>749</v>
+        <v>732</v>
       </c>
     </row>
     <row r="167" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A167" s="0" t="s">
-        <v>750</v>
+        <v>733</v>
       </c>
     </row>
     <row r="168" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A168" s="0" t="s">
-        <v>751</v>
+        <v>734</v>
       </c>
     </row>
     <row r="169" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A169" s="0" t="s">
-        <v>752</v>
+        <v>735</v>
       </c>
     </row>
     <row r="170" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A170" s="0" t="s">
-        <v>753</v>
+        <v>736</v>
       </c>
     </row>
     <row r="171" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A171" s="0" t="s">
-        <v>754</v>
+        <v>737</v>
       </c>
     </row>
     <row r="172" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A172" s="0" t="s">
-        <v>755</v>
+        <v>738</v>
       </c>
     </row>
     <row r="173" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A173" s="0" t="s">
-        <v>756</v>
+        <v>739</v>
       </c>
     </row>
     <row r="174" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A174" s="0" t="s">
-        <v>757</v>
+        <v>740</v>
       </c>
     </row>
     <row r="175" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A175" s="0" t="s">
-        <v>758</v>
+        <v>741</v>
       </c>
     </row>
     <row r="176" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A176" s="0" t="s">
-        <v>759</v>
+        <v>742</v>
       </c>
     </row>
     <row r="177" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A177" s="0" t="s">
-        <v>760</v>
+        <v>743</v>
       </c>
     </row>
     <row r="178" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A178" s="0" t="s">
-        <v>761</v>
+        <v>744</v>
       </c>
     </row>
     <row r="179" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A179" s="0" t="s">
-        <v>762</v>
+        <v>745</v>
       </c>
     </row>
     <row r="180" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A180" s="0" t="s">
-        <v>763</v>
+        <v>746</v>
       </c>
     </row>
     <row r="181" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A181" s="0" t="s">
-        <v>764</v>
+        <v>747</v>
       </c>
     </row>
     <row r="182" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A182" s="0" t="s">
-        <v>765</v>
+        <v>748</v>
       </c>
     </row>
     <row r="183" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A183" s="0" t="s">
-        <v>766</v>
+        <v>749</v>
       </c>
     </row>
     <row r="184" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A184" s="0" t="s">
-        <v>767</v>
+        <v>750</v>
       </c>
     </row>
     <row r="185" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A185" s="0" t="s">
-        <v>768</v>
+        <v>751</v>
       </c>
     </row>
     <row r="186" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A186" s="0" t="s">
-        <v>769</v>
+        <v>752</v>
       </c>
     </row>
     <row r="187" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A187" s="0" t="s">
-        <v>770</v>
+        <v>753</v>
       </c>
     </row>
     <row r="188" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A188" s="0" t="s">
-        <v>771</v>
+        <v>754</v>
       </c>
     </row>
     <row r="189" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A189" s="0" t="s">
-        <v>772</v>
+        <v>755</v>
       </c>
     </row>
     <row r="190" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A190" s="0" t="s">
-        <v>773</v>
+        <v>756</v>
       </c>
     </row>
     <row r="191" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A191" s="0" t="s">
-        <v>774</v>
+        <v>757</v>
       </c>
     </row>
     <row r="192" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A192" s="0" t="s">
-        <v>775</v>
+        <v>758</v>
       </c>
     </row>
     <row r="193" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A193" s="0" t="s">
-        <v>776</v>
+        <v>759</v>
       </c>
     </row>
     <row r="194" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A194" s="0" t="s">
-        <v>777</v>
+        <v>760</v>
       </c>
     </row>
     <row r="195" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A195" s="0" t="s">
-        <v>778</v>
+        <v>761</v>
       </c>
     </row>
     <row r="196" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A196" s="0" t="s">
-        <v>779</v>
+        <v>762</v>
       </c>
     </row>
     <row r="197" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A197" s="0" t="s">
-        <v>780</v>
+        <v>763</v>
       </c>
     </row>
     <row r="198" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A198" s="0" t="s">
-        <v>781</v>
+        <v>764</v>
       </c>
     </row>
     <row r="199" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A199" s="0" t="s">
-        <v>782</v>
+        <v>765</v>
       </c>
     </row>
     <row r="200" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A200" s="0" t="s">
-        <v>783</v>
+        <v>766</v>
       </c>
     </row>
     <row r="201" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A201" s="0" t="s">
-        <v>784</v>
+        <v>767</v>
       </c>
     </row>
     <row r="202" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A202" s="0" t="s">
-        <v>785</v>
+        <v>768</v>
       </c>
     </row>
     <row r="203" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A203" s="0" t="s">
-        <v>786</v>
+        <v>769</v>
       </c>
     </row>
     <row r="204" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A204" s="0" t="s">
-        <v>787</v>
+        <v>770</v>
       </c>
     </row>
     <row r="205" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A205" s="0" t="s">
-        <v>788</v>
+        <v>771</v>
       </c>
     </row>
     <row r="206" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A206" s="0" t="s">
-        <v>789</v>
+        <v>772</v>
       </c>
     </row>
     <row r="207" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A207" s="0" t="s">
-        <v>790</v>
+        <v>773</v>
       </c>
     </row>
     <row r="208" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A208" s="0" t="s">
-        <v>791</v>
+        <v>774</v>
       </c>
     </row>
     <row r="209" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A209" s="0" t="s">
-        <v>792</v>
+        <v>775</v>
       </c>
     </row>
     <row r="210" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A210" s="0" t="s">
-        <v>793</v>
+        <v>776</v>
       </c>
     </row>
     <row r="211" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A211" s="0" t="s">
-        <v>794</v>
+        <v>777</v>
       </c>
     </row>
     <row r="212" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A212" s="0" t="s">
-        <v>795</v>
+        <v>778</v>
       </c>
     </row>
     <row r="213" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A213" s="0" t="s">
-        <v>796</v>
+        <v>779</v>
       </c>
     </row>
     <row r="214" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A214" s="0" t="s">
-        <v>797</v>
+        <v>780</v>
       </c>
     </row>
     <row r="215" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A215" s="0" t="s">
-        <v>798</v>
+        <v>781</v>
       </c>
     </row>
     <row r="216" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A216" s="0" t="s">
-        <v>799</v>
+        <v>782</v>
       </c>
     </row>
     <row r="217" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A217" s="0" t="s">
-        <v>800</v>
+        <v>783</v>
       </c>
     </row>
     <row r="218" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A218" s="0" t="s">
-        <v>801</v>
+        <v>784</v>
       </c>
     </row>
     <row r="219" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A219" s="0" t="s">
-        <v>802</v>
+        <v>785</v>
       </c>
     </row>
     <row r="220" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A220" s="0" t="s">
-        <v>803</v>
+        <v>786</v>
       </c>
     </row>
     <row r="221" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A221" s="0" t="s">
-        <v>804</v>
+        <v>787</v>
       </c>
     </row>
     <row r="222" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A222" s="0" t="s">
-        <v>805</v>
+        <v>788</v>
       </c>
     </row>
     <row r="223" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A223" s="0" t="s">
-        <v>806</v>
+        <v>789</v>
       </c>
     </row>
     <row r="224" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A224" s="0" t="s">
-        <v>807</v>
+        <v>790</v>
       </c>
     </row>
     <row r="225" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A225" s="0" t="s">
-        <v>808</v>
+        <v>791</v>
       </c>
     </row>
     <row r="226" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A226" s="0" t="s">
-        <v>809</v>
+        <v>792</v>
       </c>
     </row>
     <row r="227" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A227" s="0" t="s">
-        <v>810</v>
+        <v>793</v>
       </c>
     </row>
     <row r="228" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A228" s="0" t="s">
-        <v>811</v>
+        <v>794</v>
       </c>
     </row>
     <row r="229" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A229" s="0" t="s">
-        <v>812</v>
+        <v>795</v>
       </c>
     </row>
     <row r="230" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A230" s="0" t="s">
-        <v>813</v>
+        <v>796</v>
       </c>
     </row>
     <row r="231" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A231" s="0" t="s">
-        <v>814</v>
+        <v>797</v>
       </c>
     </row>
     <row r="232" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A232" s="0" t="s">
-        <v>815</v>
+        <v>798</v>
       </c>
     </row>
     <row r="233" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A233" s="0" t="s">
-        <v>816</v>
+        <v>799</v>
       </c>
     </row>
     <row r="234" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A234" s="0" t="s">
-        <v>817</v>
+        <v>800</v>
       </c>
     </row>
     <row r="235" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A235" s="0" t="s">
-        <v>818</v>
+        <v>801</v>
       </c>
     </row>
     <row r="236" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A236" s="0" t="s">
-        <v>819</v>
+        <v>802</v>
       </c>
     </row>
     <row r="237" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A237" s="0" t="s">
-        <v>820</v>
+        <v>803</v>
       </c>
     </row>
     <row r="238" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A238" s="0" t="s">
-        <v>821</v>
+        <v>804</v>
       </c>
     </row>
     <row r="239" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A239" s="0" t="s">
-        <v>822</v>
+        <v>805</v>
       </c>
     </row>
     <row r="240" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A240" s="0" t="s">
-        <v>823</v>
+        <v>806</v>
       </c>
     </row>
     <row r="241" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A241" s="0" t="s">
-        <v>824</v>
+        <v>807</v>
       </c>
     </row>
     <row r="242" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A242" s="0" t="s">
-        <v>825</v>
+        <v>808</v>
       </c>
     </row>
     <row r="243" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A243" s="0" t="s">
-        <v>826</v>
+        <v>809</v>
       </c>
     </row>
     <row r="244" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A244" s="0" t="s">
-        <v>827</v>
+        <v>810</v>
       </c>
     </row>
     <row r="245" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A245" s="0" t="s">
-        <v>828</v>
+        <v>811</v>
       </c>
     </row>
     <row r="246" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A246" s="0" t="s">
-        <v>829</v>
+        <v>812</v>
       </c>
     </row>
     <row r="247" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A247" s="0" t="s">
-        <v>830</v>
+        <v>813</v>
       </c>
     </row>
     <row r="248" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A248" s="0" t="s">
-        <v>831</v>
+        <v>814</v>
       </c>
     </row>
     <row r="249" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A249" s="0" t="s">
-        <v>832</v>
+        <v>815</v>
       </c>
     </row>
   </sheetData>
@@ -14195,7 +13428,7 @@
   <dimension ref="A1:P32"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+      <selection pane="topLeft" activeCell="B4" activeCellId="0" sqref="B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -15636,10 +14869,6 @@
       <formula1>"PUBLIC,PRIVATE,DISPUTED"</formula1>
       <formula2>0</formula2>
     </dataValidation>
-    <dataValidation allowBlank="true" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="C5:C33" type="list">
-      <formula1>"Nonprofit/NGO ,Foundation/Philanthropist,Government/Public Sector/Public Bank ,Multilateral/Bilateral/Intergovernmental Financial Institution,Corporate Giving ,Investment Fund,High Net Worth Individual/Family Office/Private Bank,Impact Investor ,Commercia"</formula1>
-      <formula2>0</formula2>
-    </dataValidation>
     <dataValidation allowBlank="true" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="L5:L33" type="list">
       <formula1>"IRR,Average annual return"</formula1>
       <formula2>0</formula2>
@@ -15652,6 +14881,10 @@
       <formula1>"Debt,Equity,Combination"</formula1>
       <formula2>0</formula2>
     </dataValidation>
+    <dataValidation allowBlank="true" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="C5:C33" type="list">
+      <formula1>InvestmentsOrgRoleOptions!$A$1:$A$9</formula1>
+      <formula2>0</formula2>
+    </dataValidation>
   </dataValidations>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>

</xml_diff>